<commit_message>
added comp_mor_ev_data to functions.py
</commit_message>
<xml_diff>
--- a/downloads/weather_data.xlsx
+++ b/downloads/weather_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,81 +443,251 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>15-01-2024</t>
+          <t>01-01-2024</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.01173135699545329</v>
+        <v>0.2640727228724609</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>16-01-2024</t>
+          <t>02-01-2024</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.08389218667816668</v>
+        <v>0.0002728733781852322</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>17-01-2024</t>
+          <t>03-01-2024</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.008029626214607797</v>
+        <v>0.01318142747795677</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>18-01-2024</t>
+          <t>04-01-2024</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.001148125312265952</v>
+        <v>0.02769346615424148</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>19-01-2024</t>
+          <t>05-01-2024</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.3920495730652868</v>
+        <v>0.1045413447121037</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>20-01-2024</t>
+          <t>06-01-2024</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.16301139171748</v>
+        <v>0.03146386253696185</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>21-01-2024</t>
+          <t>07-01-2024</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4922478884896943</v>
+        <v>0.003810482642393739</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>08-01-2024</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5208876517689147</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>09-01-2024</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.9372133312270073</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>10-01-2024</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.8436036806890808</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>11-01-2024</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.8617712033086313</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>12-01-2024</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.02167194237400416</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>13-01-2024</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.02033969313737993</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>14-01-2024</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.01212794262982757</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>15-01-2024</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.01173135699545329</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>16-01-2024</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.08389218667816668</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>17-01-2024</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.008029626214607797</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>18-01-2024</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.001148125312265952</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>19-01-2024</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.3920495730652868</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>20-01-2024</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1.16301139171748</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>21-01-2024</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.4922478884896943</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
           <t>22-01-2024</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B23" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>23-01-2024</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.4999612913260334</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>24-01-2024</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.2215556335889916</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>25-01-2024</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.3556320059476869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>